<commit_message>
It open the data_2.txt and it replaces the text. Instead of comma we now have points
</commit_message>
<xml_diff>
--- a/phases.xlsx
+++ b/phases.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B7FC325-7E09-48C5-9CCA-E27006B79753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6573DB52-DD64-4765-89B8-B06E70BCEC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -19,6 +19,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -950,7 +952,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -990,7 +992,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1306,8 +1308,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:AD277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6685,7 +6687,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6693,21 +6697,10 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100BA85B17551307B4383D2980D4EFA5515" ma:contentTypeVersion="12" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="57aaa53a121281638ac8bc132f802243">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="173d6b2f-59a8-488e-935d-67e78bda59e5" xmlns:ns3="b97dc65e-fe16-4df7-925c-ff3316bf7bf3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="141727366efbfc4d0736cea1f099176a" ns2:_="" ns3:_="">
     <xsd:import namespace="173d6b2f-59a8-488e-935d-67e78bda59e5"/>
@@ -6924,9 +6917,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
-  <ds:schemaRefs/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BD3FF0-C90B-4BBB-AF14-2B7944CED71E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fe0e463f-46c1-4b5a-aeae-2e65b5901510"/>
+  </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
@@ -6937,24 +6943,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BD3FF0-C90B-4BBB-AF14-2B7944CED71E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fe0e463f-46c1-4b5a-aeae-2e65b5901510"/>
-  </ds:schemaRefs>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
+  <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{754B3D83-15E4-4B5F-8568-57884EBAF882}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6971,4 +6965,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
It replaces the text of a single line. Next: should process all the lines in data_2.txt
</commit_message>
<xml_diff>
--- a/phases.xlsx
+++ b/phases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6573DB52-DD64-4765-89B8-B06E70BCEC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D0387B-FEAC-4089-A967-B063FF10441C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="289">
   <si>
     <t>BG2,X,Force,1000000</t>
   </si>
@@ -932,12 +932,6 @@
     <t>BG10</t>
   </si>
   <si>
-    <t>Phase 1: paste from python file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase 2: paste from </t>
-  </si>
-  <si>
     <t>Phase 3: put the values you would like</t>
   </si>
   <si>
@@ -945,6 +939,9 @@
   </si>
   <si>
     <t>Phase 5</t>
+  </si>
+  <si>
+    <t>Phase 1: paste from output.csv</t>
   </si>
 </sst>
 </file>
@@ -1308,8 +1305,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:AD277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1330,19 +1327,16 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>288</v>
+      </c>
+      <c r="P1" t="s">
         <v>285</v>
       </c>
-      <c r="H1" t="s">
+      <c r="X1" t="s">
         <v>286</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AD1" t="s">
         <v>287</v>
-      </c>
-      <c r="X1" t="s">
-        <v>288</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -6687,9 +6681,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6697,10 +6689,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100BA85B17551307B4383D2980D4EFA5515" ma:contentTypeVersion="12" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="57aaa53a121281638ac8bc132f802243">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="173d6b2f-59a8-488e-935d-67e78bda59e5" xmlns:ns3="b97dc65e-fe16-4df7-925c-ff3316bf7bf3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="141727366efbfc4d0736cea1f099176a" ns2:_="" ns3:_="">
     <xsd:import namespace="173d6b2f-59a8-488e-935d-67e78bda59e5"/>
@@ -6917,22 +6920,9 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BD3FF0-C90B-4BBB-AF14-2B7944CED71E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fe0e463f-46c1-4b5a-aeae-2e65b5901510"/>
-  </ds:schemaRefs>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
+  <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
@@ -6943,12 +6933,24 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
-  <ds:schemaRefs/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BD3FF0-C90B-4BBB-AF14-2B7944CED71E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fe0e463f-46c1-4b5a-aeae-2e65b5901510"/>
+  </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{754B3D83-15E4-4B5F-8568-57884EBAF882}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6965,12 +6967,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
It works with "Force" and "Moment"
</commit_message>
<xml_diff>
--- a/phases.xlsx
+++ b/phases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BACF7C1-EF70-4A06-8406-05A0E983D007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F42989-9777-48E1-A738-0F19D1B932C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1313,7 +1313,7 @@
   <dimension ref="A1:AD278"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1396,13 +1396,13 @@
         <v>176</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>174</v>
+        <v>281</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>175</v>
+        <v>282</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>176</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -1485,11 +1485,11 @@
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="1"/>
-        <v>BG7;X;-1197725;Moment</v>
+        <v>BG7;Mx;-1197725;Moment</v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>BG7;Y;11,5;Moment</v>
+        <v>BG7;My;11,5;Moment</v>
       </c>
       <c r="AD4" t="str" cm="1">
         <f t="array" ref="AD4:AD23">_xlfn.TOCOL(X4:AB7)</f>
@@ -1576,11 +1576,11 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" ref="AA5:AA7" si="6">_xlfn.CONCAT($P5, ";", T$3, ";",T5,";",T$2)</f>
-        <v>BG8;X;1191630;Moment</v>
+        <v>BG8;Mx;1191630;Moment</v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" ref="AB5:AB7" si="7">_xlfn.CONCAT($P5, ";", U$3, ";",U5,";",U$2)</f>
-        <v>BG8;Y;11,5;Moment</v>
+        <v>BG8;My;11,5;Moment</v>
       </c>
       <c r="AD5" t="str">
         <v>BG7;Y;464025;Force</v>
@@ -1666,11 +1666,11 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="6"/>
-        <v>BG9;X;-349715;Moment</v>
+        <v>BG9;Mx;-349715;Moment</v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="7"/>
-        <v>BG9;Y;1,15;Moment</v>
+        <v>BG9;My;1,15;Moment</v>
       </c>
       <c r="AD6" t="str">
         <v>BG7;Z;-1392535;Force</v>
@@ -1756,14 +1756,14 @@
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="6"/>
-        <v>BG10;X;360984,9885;Moment</v>
+        <v>BG10;Mx;360984,9885;Moment</v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="7"/>
-        <v>BG10;Y;1,15;Moment</v>
+        <v>BG10;My;1,15;Moment</v>
       </c>
       <c r="AD7" t="str">
-        <v>BG7;X;-1197725;Moment</v>
+        <v>BG7;Mx;-1197725;Moment</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -1784,7 +1784,7 @@
         <v>403500</v>
       </c>
       <c r="AD8" t="str">
-        <v>BG7;Y;11,5;Moment</v>
+        <v>BG7;My;11,5;Moment</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
@@ -1868,7 +1868,7 @@
         <v>-2026000</v>
       </c>
       <c r="AD12" t="str">
-        <v>BG8;X;1191630;Moment</v>
+        <v>BG8;Mx;1191630;Moment</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
@@ -1889,7 +1889,7 @@
         <v>1</v>
       </c>
       <c r="AD13" t="str">
-        <v>BG8;Y;11,5;Moment</v>
+        <v>BG8;My;11,5;Moment</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
@@ -1973,7 +1973,7 @@
         <v>-191500</v>
       </c>
       <c r="AD17" t="str">
-        <v>BG9;X;-349715;Moment</v>
+        <v>BG9;Mx;-349715;Moment</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
@@ -1994,7 +1994,7 @@
         <v>-2519900</v>
       </c>
       <c r="AD18" t="str">
-        <v>BG9;Y;1,15;Moment</v>
+        <v>BG9;My;1,15;Moment</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
@@ -2078,7 +2078,7 @@
         <v>1</v>
       </c>
       <c r="AD22" t="str">
-        <v>BG10;X;360984,9885;Moment</v>
+        <v>BG10;Mx;360984,9885;Moment</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
@@ -2099,7 +2099,7 @@
         <v>147900</v>
       </c>
       <c r="AD23" t="str">
-        <v>BG10;Y;1,15;Moment</v>
+        <v>BG10;My;1,15;Moment</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
@@ -6708,10 +6708,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
+<TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100BA85B17551307B4383D2980D4EFA5515" ma:contentTypeVersion="12" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="57aaa53a121281638ac8bc132f802243">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="173d6b2f-59a8-488e-935d-67e78bda59e5" xmlns:ns3="b97dc65e-fe16-4df7-925c-ff3316bf7bf3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="141727366efbfc4d0736cea1f099176a" ns2:_="" ns3:_="">
     <xsd:import namespace="173d6b2f-59a8-488e-935d-67e78bda59e5"/>
@@ -6928,32 +6943,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
+<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69C2894E-68C9-476D-803E-814AC6EBDDB7}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BD3FF0-C90B-4BBB-AF14-2B7944CED71E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fe0e463f-46c1-4b5a-aeae-2e65b5901510"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{754B3D83-15E4-4B5F-8568-57884EBAF882}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6972,26 +6990,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BD3FF0-C90B-4BBB-AF14-2B7944CED71E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fe0e463f-46c1-4b5a-aeae-2e65b5901510"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69C2894E-68C9-476D-803E-814AC6EBDDB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
First version that works. I should clean the files
</commit_message>
<xml_diff>
--- a/phases.xlsx
+++ b/phases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F42989-9777-48E1-A738-0F19D1B932C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57E010A-9C9C-40DD-B6A5-5C8719CEB990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>BG7,X,Force,1</t>
   </si>
   <si>
-    <t>BG7,Y,Force,403500</t>
-  </si>
-  <si>
     <t>BG7,Z,Force,-1210900</t>
   </si>
   <si>
@@ -929,25 +926,28 @@
     <t>Mz</t>
   </si>
   <si>
+    <t>Phase 3: put the values you would like</t>
+  </si>
+  <si>
+    <t>Phase 4</t>
+  </si>
+  <si>
+    <t>Phase 5</t>
+  </si>
+  <si>
+    <t>Phase 1: paste from output.csv</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Moment</t>
+  </si>
+  <si>
+    <t>BG7,Y,Force,-1224690</t>
+  </si>
+  <si>
     <t>BG10</t>
-  </si>
-  <si>
-    <t>Phase 3: put the values you would like</t>
-  </si>
-  <si>
-    <t>Phase 4</t>
-  </si>
-  <si>
-    <t>Phase 5</t>
-  </si>
-  <si>
-    <t>Phase 1: paste from output.csv</t>
-  </si>
-  <si>
-    <t>Force</t>
-  </si>
-  <si>
-    <t>Moment</t>
   </si>
 </sst>
 </file>
@@ -989,14 +989,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1310,10 +1309,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Blad1"/>
-  <dimension ref="A1:AD278"/>
+  <dimension ref="A1:AE278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1329,83 +1328,84 @@
     <col min="27" max="27" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.28515625" customWidth="1"/>
+    <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>286</v>
+      </c>
+      <c r="P1" t="s">
+        <v>283</v>
+      </c>
+      <c r="X1" t="s">
+        <v>284</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="Q2" t="s">
+        <v>287</v>
+      </c>
+      <c r="R2" t="s">
+        <v>287</v>
+      </c>
+      <c r="S2" t="s">
+        <v>287</v>
+      </c>
+      <c r="T2" t="s">
         <v>288</v>
       </c>
-      <c r="P1" t="s">
-        <v>285</v>
-      </c>
-      <c r="X1" t="s">
-        <v>286</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="Q2" t="s">
-        <v>289</v>
-      </c>
-      <c r="R2" t="s">
-        <v>289</v>
-      </c>
-      <c r="S2" t="s">
-        <v>289</v>
-      </c>
-      <c r="T2" t="s">
-        <v>290</v>
-      </c>
       <c r="U2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="V2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J3" t="s">
         <v>174</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>175</v>
       </c>
-      <c r="K3" t="s">
-        <v>176</v>
-      </c>
       <c r="L3" t="s">
+        <v>280</v>
+      </c>
+      <c r="M3" t="s">
         <v>281</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>282</v>
-      </c>
-      <c r="N3" t="s">
-        <v>283</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="T3" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>1000000</v>
       </c>
       <c r="H4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I4" t="str" cm="1">
         <f t="array" ref="I4">_xlfn.DROP(_xlfn._xlws.FILTER($B$4:$E$278, ($B$4:$B$278=$H4)*( $C$4:$C$278=I$3)), ,3)</f>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="J4" t="str" cm="1">
         <f t="array" ref="J4">_xlfn.DROP(_xlfn._xlws.FILTER($B$4:$E$278, ($B$4:$B$278=$H4)*( $C$4:$C$278=J$3)), ,3)</f>
-        <v>403500</v>
+        <v>-1224690</v>
       </c>
       <c r="K4" t="str" cm="1">
         <f t="array" ref="K4">_xlfn.DROP(_xlfn._xlws.FILTER($B$4:$E$278, ($B$4:$B$278=$H4)*( $C$4:$C$278=K$3)), ,3)</f>
@@ -1450,53 +1450,53 @@
         <v>#VALUE!</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>1.1499999999999999</v>
+        <v>172</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.1</v>
       </c>
       <c r="R4" s="3">
-        <v>464024.99999999994</v>
+        <v>-1224.69</v>
       </c>
       <c r="S4" s="3">
-        <v>-1392535</v>
+        <v>-3475.21</v>
       </c>
       <c r="T4" s="3">
-        <v>-1197725</v>
+        <v>0.1</v>
       </c>
       <c r="U4" s="3">
-        <v>11.5</v>
+        <v>0.1</v>
       </c>
       <c r="V4" s="2" t="e" vm="2">
         <f t="shared" ref="V4" si="0">N4*1.15</f>
         <v>#VALUE!</v>
       </c>
       <c r="X4" t="str">
-        <f>_xlfn.CONCAT($P4, ";", Q$3, ";",Q4,";",Q$2)</f>
-        <v>BG7;X;1,15;Force</v>
+        <f>_xlfn.CONCAT($P4, ";", Q$3, ";",Q4*1000,";",Q$2)</f>
+        <v>BG7;X;100;Force</v>
       </c>
       <c r="Y4" t="str">
-        <f t="shared" ref="Y4:AB4" si="1">_xlfn.CONCAT($P4, ";", R$3, ";",R4,";",R$2)</f>
-        <v>BG7;Y;464025;Force</v>
+        <f t="shared" ref="Y4:AB4" si="1">_xlfn.CONCAT($P4, ";", R$3, ";",R4*1000,";",R$2)</f>
+        <v>BG7;Y;-1224690;Force</v>
       </c>
       <c r="Z4" t="str">
         <f t="shared" si="1"/>
-        <v>BG7;Z;-1392535;Force</v>
+        <v>BG7;Z;-3475210;Force</v>
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="1"/>
-        <v>BG7;Mx;-1197725;Moment</v>
+        <v>BG7;Mx;100;Moment</v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>BG7;My;11,5;Moment</v>
-      </c>
-      <c r="AD4" t="str" cm="1">
-        <f t="array" ref="AD4:AD23">_xlfn.TOCOL(X4:AB7)</f>
-        <v>BG7;X;1,15;Force</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+        <v>BG7;My;100;Moment</v>
+      </c>
+      <c r="AE4" t="str" cm="1">
+        <f t="array" ref="AE4:AE83">_xlfn.TOCOL(X4:AB19)</f>
+        <v>BG7;X;100;Force</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>1000000</v>
       </c>
       <c r="H5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I5" t="str" cm="1">
         <f t="array" ref="I5">_xlfn.DROP(_xlfn._xlws.FILTER($B$4:$E$278, ($B$4:$B$278=$H5)*( $C$4:$C$278=I$3)), ,3)</f>
@@ -1541,52 +1541,52 @@
         <v>#VALUE!</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>1.1499999999999999</v>
+        <v>176</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.1</v>
       </c>
       <c r="R5" s="3">
-        <v>-467129.99999999994</v>
+        <v>751.04</v>
       </c>
       <c r="S5" s="3">
-        <v>-2329900</v>
+        <v>8183.65</v>
       </c>
       <c r="T5" s="3">
-        <v>1191630</v>
+        <v>0.1</v>
       </c>
       <c r="U5" s="3">
-        <v>11.5</v>
+        <v>0.1</v>
       </c>
       <c r="V5" s="2" t="e" vm="2">
-        <f t="shared" ref="V5:V7" si="2">N5*1.15</f>
+        <f t="shared" ref="V5:V6" si="2">N5*1.15</f>
         <v>#VALUE!</v>
       </c>
       <c r="X5" t="str">
-        <f t="shared" ref="X5:X7" si="3">_xlfn.CONCAT($P5, ";", Q$3, ";",Q5,";",Q$2)</f>
-        <v>BG8;X;1,15;Force</v>
+        <f t="shared" ref="X5:X11" si="3">_xlfn.CONCAT($P5, ";", Q$3, ";",Q5*1000,";",Q$2)</f>
+        <v>BG8;X;100;Force</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" ref="Y5:Y7" si="4">_xlfn.CONCAT($P5, ";", R$3, ";",R5,";",R$2)</f>
-        <v>BG8;Y;-467130;Force</v>
+        <f t="shared" ref="Y5:Y11" si="4">_xlfn.CONCAT($P5, ";", R$3, ";",R5*1000,";",R$2)</f>
+        <v>BG8;Y;751040;Force</v>
       </c>
       <c r="Z5" t="str">
-        <f t="shared" ref="Z5:Z7" si="5">_xlfn.CONCAT($P5, ";", S$3, ";",S5,";",S$2)</f>
-        <v>BG8;Z;-2329900;Force</v>
+        <f t="shared" ref="Z5:Z11" si="5">_xlfn.CONCAT($P5, ";", S$3, ";",S5*1000,";",S$2)</f>
+        <v>BG8;Z;8183650;Force</v>
       </c>
       <c r="AA5" t="str">
-        <f t="shared" ref="AA5:AA7" si="6">_xlfn.CONCAT($P5, ";", T$3, ";",T5,";",T$2)</f>
-        <v>BG8;Mx;1191630;Moment</v>
+        <f t="shared" ref="AA5:AA11" si="6">_xlfn.CONCAT($P5, ";", T$3, ";",T5*1000,";",T$2)</f>
+        <v>BG8;Mx;100;Moment</v>
       </c>
       <c r="AB5" t="str">
-        <f t="shared" ref="AB5:AB7" si="7">_xlfn.CONCAT($P5, ";", U$3, ";",U5,";",U$2)</f>
-        <v>BG8;My;11,5;Moment</v>
-      </c>
-      <c r="AD5" t="str">
-        <v>BG7;Y;464025;Force</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+        <f t="shared" ref="AB5:AB11" si="7">_xlfn.CONCAT($P5, ";", U$3, ";",U5*1000,";",U$2)</f>
+        <v>BG8;My;100;Moment</v>
+      </c>
+      <c r="AE5" t="str">
+        <v>BG7;Y;-1224690;Force</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>-1000000</v>
       </c>
       <c r="H6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I6" t="str" cm="1">
         <f t="array" ref="I6">_xlfn.DROP(_xlfn._xlws.FILTER($B$4:$E$278, ($B$4:$B$278=$H6)*( $C$4:$C$278=I$3)), ,3)</f>
@@ -1631,22 +1631,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>1.1499999999999999</v>
+        <v>177</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.1</v>
       </c>
       <c r="R6" s="3">
-        <v>226434.99999999997</v>
+        <v>-1030.01</v>
       </c>
       <c r="S6" s="3">
-        <v>-1183695</v>
+        <v>-3808.5</v>
       </c>
       <c r="T6" s="3">
-        <v>-349715</v>
+        <v>0.1</v>
       </c>
       <c r="U6" s="3">
-        <v>1.1499999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="V6" s="2" t="e" vm="2">
         <f t="shared" si="2"/>
@@ -1654,29 +1654,29 @@
       </c>
       <c r="X6" t="str">
         <f t="shared" si="3"/>
-        <v>BG9;X;1,15;Force</v>
+        <v>BG9;X;100;Force</v>
       </c>
       <c r="Y6" t="str">
         <f t="shared" si="4"/>
-        <v>BG9;Y;226435;Force</v>
+        <v>BG9;Y;-1030010;Force</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" si="5"/>
-        <v>BG9;Z;-1183695;Force</v>
+        <v>BG9;Z;-3808500;Force</v>
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="6"/>
-        <v>BG9;Mx;-349715;Moment</v>
+        <v>BG9;Mx;100;Moment</v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="7"/>
-        <v>BG9;My;1,15;Moment</v>
-      </c>
-      <c r="AD6" t="str">
-        <v>BG7;Z;-1392535;Force</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+        <v>BG9;My;100;Moment</v>
+      </c>
+      <c r="AE6" t="str">
+        <v>BG7;Z;-3475210;Force</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="I7" t="str" cm="1">
         <f t="array" ref="I7">_xlfn.DROP(_xlfn._xlws.FILTER($B$4:$E$278, ($B$4:$B$278=$H7)*( $C$4:$C$278=I$3)), ,3)</f>
@@ -1721,54 +1721,51 @@
         <v>#VALUE!</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>1.1499999999999999</v>
+        <v>290</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0.1</v>
       </c>
       <c r="R7" s="3">
-        <v>-220224.99999999997</v>
+        <v>556.36</v>
       </c>
       <c r="S7" s="3">
-        <v>-2897885</v>
+        <v>8516.9500000000007</v>
       </c>
       <c r="T7" s="3">
-        <v>360984.98849999998</v>
+        <v>0.1</v>
       </c>
       <c r="U7" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="V7" s="2" t="e" vm="2">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="V7" s="2"/>
       <c r="X7" t="str">
         <f t="shared" si="3"/>
-        <v>BG10;X;1,15;Force</v>
+        <v>BG10;X;100;Force</v>
       </c>
       <c r="Y7" t="str">
         <f t="shared" si="4"/>
-        <v>BG10;Y;-220225;Force</v>
+        <v>BG10;Y;556360;Force</v>
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="5"/>
-        <v>BG10;Z;-2897885;Force</v>
+        <v>BG10;Z;8516950;Force</v>
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="6"/>
-        <v>BG10;Mx;360984,9885;Moment</v>
+        <v>BG10;Mx;100;Moment</v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="7"/>
-        <v>BG10;My;1,15;Moment</v>
-      </c>
-      <c r="AD7" t="str">
-        <v>BG7;Mx;-1197725;Moment</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+        <v>BG10;My;100;Moment</v>
+      </c>
+      <c r="AE7" t="str">
+        <v>BG7;Mx;100;Moment</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>289</v>
       </c>
       <c r="B8" t="str" cm="1">
         <f t="array" ref="B8:E8">_xlfn.TEXTSPLIT(A8, ",")</f>
@@ -1781,15 +1778,36 @@
         <v>Force</v>
       </c>
       <c r="E8" t="str">
-        <v>403500</v>
-      </c>
-      <c r="AD8" t="str">
-        <v>BG7;My;11,5;Moment</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+        <v>-1224690</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="X8" t="str">
+        <f t="shared" si="3"/>
+        <v>;X;0;Force</v>
+      </c>
+      <c r="Y8" t="str">
+        <f t="shared" si="4"/>
+        <v>;Y;0;Force</v>
+      </c>
+      <c r="Z8" t="str">
+        <f t="shared" si="5"/>
+        <v>;Z;0;Force</v>
+      </c>
+      <c r="AA8" t="str">
+        <f t="shared" si="6"/>
+        <v>;Mx;0;Moment</v>
+      </c>
+      <c r="AB8" t="str">
+        <f t="shared" si="7"/>
+        <v>;My;0;Moment</v>
+      </c>
+      <c r="AE8" t="str">
+        <v>BG7;My;100;Moment</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="str" cm="1">
         <f t="array" ref="B9:E9">_xlfn.TEXTSPLIT(A9, ",")</f>
@@ -1804,13 +1822,34 @@
       <c r="E9" t="str">
         <v>-1210900</v>
       </c>
-      <c r="AD9" t="str">
-        <v>BG8;X;1,15;Force</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="P9" s="2"/>
+      <c r="X9" t="str">
+        <f t="shared" si="3"/>
+        <v>;X;0;Force</v>
+      </c>
+      <c r="Y9" t="str">
+        <f t="shared" si="4"/>
+        <v>;Y;0;Force</v>
+      </c>
+      <c r="Z9" t="str">
+        <f t="shared" si="5"/>
+        <v>;Z;0;Force</v>
+      </c>
+      <c r="AA9" t="str">
+        <f t="shared" si="6"/>
+        <v>;Mx;0;Moment</v>
+      </c>
+      <c r="AB9" t="str">
+        <f t="shared" si="7"/>
+        <v>;My;0;Moment</v>
+      </c>
+      <c r="AE9" t="str">
+        <v>BG8;X;100;Force</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:E10">_xlfn.TEXTSPLIT(A10, ",")</f>
@@ -1825,13 +1864,34 @@
       <c r="E10" t="str">
         <v>1</v>
       </c>
-      <c r="AD10" t="str">
-        <v>BG8;Y;-467130;Force</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="P10" s="2"/>
+      <c r="X10" t="str">
+        <f t="shared" si="3"/>
+        <v>;X;0;Force</v>
+      </c>
+      <c r="Y10" t="str">
+        <f t="shared" si="4"/>
+        <v>;Y;0;Force</v>
+      </c>
+      <c r="Z10" t="str">
+        <f t="shared" si="5"/>
+        <v>;Z;0;Force</v>
+      </c>
+      <c r="AA10" t="str">
+        <f t="shared" si="6"/>
+        <v>;Mx;0;Moment</v>
+      </c>
+      <c r="AB10" t="str">
+        <f t="shared" si="7"/>
+        <v>;My;0;Moment</v>
+      </c>
+      <c r="AE10" t="str">
+        <v>BG8;Y;751040;Force</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="str" cm="1">
         <f t="array" ref="B11:E11">_xlfn.TEXTSPLIT(A11, ",")</f>
@@ -1846,13 +1906,34 @@
       <c r="E11" t="str">
         <v>-406200</v>
       </c>
-      <c r="AD11" t="str">
-        <v>BG8;Z;-2329900;Force</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="P11" s="2"/>
+      <c r="X11" t="str">
+        <f t="shared" si="3"/>
+        <v>;X;0;Force</v>
+      </c>
+      <c r="Y11" t="str">
+        <f t="shared" si="4"/>
+        <v>;Y;0;Force</v>
+      </c>
+      <c r="Z11" t="str">
+        <f t="shared" si="5"/>
+        <v>;Z;0;Force</v>
+      </c>
+      <c r="AA11" t="str">
+        <f t="shared" si="6"/>
+        <v>;Mx;0;Moment</v>
+      </c>
+      <c r="AB11" t="str">
+        <f t="shared" si="7"/>
+        <v>;My;0;Moment</v>
+      </c>
+      <c r="AE11" t="str">
+        <v>BG8;Z;8183650;Force</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="str" cm="1">
         <f t="array" ref="B12:E12">_xlfn.TEXTSPLIT(A12, ",")</f>
@@ -1867,13 +1948,13 @@
       <c r="E12" t="str">
         <v>-2026000</v>
       </c>
-      <c r="AD12" t="str">
-        <v>BG8;Mx;1191630;Moment</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE12" t="str">
+        <v>BG8;Mx;100;Moment</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="str" cm="1">
         <f t="array" ref="B13:E13">_xlfn.TEXTSPLIT(A13, ",")</f>
@@ -1888,13 +1969,13 @@
       <c r="E13" t="str">
         <v>1</v>
       </c>
-      <c r="AD13" t="str">
-        <v>BG8;My;11,5;Moment</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE13" t="str">
+        <v>BG8;My;100;Moment</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="str" cm="1">
         <f t="array" ref="B14:E14">_xlfn.TEXTSPLIT(A14, ",")</f>
@@ -1909,13 +1990,13 @@
       <c r="E14" t="str">
         <v>196900</v>
       </c>
-      <c r="AD14" t="str">
-        <v>BG9;X;1,15;Force</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE14" t="str">
+        <v>BG9;X;100;Force</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="str" cm="1">
         <f t="array" ref="B15:E15">_xlfn.TEXTSPLIT(A15, ",")</f>
@@ -1930,13 +2011,13 @@
       <c r="E15" t="str">
         <v>-1029300</v>
       </c>
-      <c r="AD15" t="str">
-        <v>BG9;Y;226435;Force</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE15" t="str">
+        <v>BG9;Y;-1030010;Force</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="str" cm="1">
         <f t="array" ref="B16:E16">_xlfn.TEXTSPLIT(A16, ",")</f>
@@ -1951,13 +2032,13 @@
       <c r="E16" t="str">
         <v>1</v>
       </c>
-      <c r="AD16" t="str">
-        <v>BG9;Z;-1183695;Force</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE16" t="str">
+        <v>BG9;Z;-3808500;Force</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" t="str" cm="1">
         <f t="array" ref="B17:E17">_xlfn.TEXTSPLIT(A17, ",")</f>
@@ -1972,13 +2053,13 @@
       <c r="E17" t="str">
         <v>-191500</v>
       </c>
-      <c r="AD17" t="str">
-        <v>BG9;Mx;-349715;Moment</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE17" t="str">
+        <v>BG9;Mx;100;Moment</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="str" cm="1">
         <f t="array" ref="B18:E18">_xlfn.TEXTSPLIT(A18, ",")</f>
@@ -1993,13 +2074,13 @@
       <c r="E18" t="str">
         <v>-2519900</v>
       </c>
-      <c r="AD18" t="str">
-        <v>BG9;My;1,15;Moment</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE18" t="str">
+        <v>BG9;My;100;Moment</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" t="str" cm="1">
         <f t="array" ref="B19:E19">_xlfn.TEXTSPLIT(A19, ",")</f>
@@ -2014,13 +2095,13 @@
       <c r="E19" t="str">
         <v>1</v>
       </c>
-      <c r="AD19" t="str">
-        <v>BG10;X;1,15;Force</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE19" t="str">
+        <v>BG10;X;100;Force</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" t="str" cm="1">
         <f t="array" ref="B20:E20">_xlfn.TEXTSPLIT(A20, ",")</f>
@@ -2035,13 +2116,13 @@
       <c r="E20" t="str">
         <v>-150600</v>
       </c>
-      <c r="AD20" t="str">
-        <v>BG10;Y;-220225;Force</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE20" t="str">
+        <v>BG10;Y;556360;Force</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" ref="B21:E21">_xlfn.TEXTSPLIT(A21, ",")</f>
@@ -2056,13 +2137,13 @@
       <c r="E21" t="str">
         <v>-1503800</v>
       </c>
-      <c r="AD21" t="str">
-        <v>BG10;Z;-2897885;Force</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE21" t="str">
+        <v>BG10;Z;8516950;Force</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" t="str" cm="1">
         <f t="array" ref="B22:E22">_xlfn.TEXTSPLIT(A22, ",")</f>
@@ -2077,13 +2158,13 @@
       <c r="E22" t="str">
         <v>1</v>
       </c>
-      <c r="AD22" t="str">
-        <v>BG10;Mx;360984,9885;Moment</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE22" t="str">
+        <v>BG10;Mx;100;Moment</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" t="str" cm="1">
         <f t="array" ref="B23:E23">_xlfn.TEXTSPLIT(A23, ",")</f>
@@ -2098,13 +2179,13 @@
       <c r="E23" t="str">
         <v>147900</v>
       </c>
-      <c r="AD23" t="str">
-        <v>BG10;My;1,15;Moment</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE23" t="str">
+        <v>BG10;My;100;Moment</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" t="str" cm="1">
         <f t="array" ref="B24:E24">_xlfn.TEXTSPLIT(A24, ",")</f>
@@ -2119,10 +2200,13 @@
       <c r="E24" t="str">
         <v>-2098700</v>
       </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE24" t="str">
+        <v>;X;0;Force</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" t="str" cm="1">
         <f t="array" ref="B25:E25">_xlfn.TEXTSPLIT(A25, ",")</f>
@@ -2137,10 +2221,13 @@
       <c r="E25" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE25" t="str">
+        <v>;Y;0;Force</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" t="str" cm="1">
         <f t="array" ref="B26:E26">_xlfn.TEXTSPLIT(A26, ",")</f>
@@ -2155,10 +2242,13 @@
       <c r="E26" t="str">
         <v>280000</v>
       </c>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE26" t="str">
+        <v>;Z;0;Force</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" t="str" cm="1">
         <f t="array" ref="B27:E27">_xlfn.TEXTSPLIT(A27, ",")</f>
@@ -2173,10 +2263,13 @@
       <c r="E27" t="str">
         <v>-1224300</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE27" t="str">
+        <v>;Mx;0;Moment</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" t="str" cm="1">
         <f t="array" ref="B28:E28">_xlfn.TEXTSPLIT(A28, ",")</f>
@@ -2191,10 +2284,13 @@
       <c r="E28" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE28" t="str">
+        <v>;My;0;Moment</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" t="str" cm="1">
         <f t="array" ref="B29:E29">_xlfn.TEXTSPLIT(A29, ",")</f>
@@ -2209,10 +2305,13 @@
       <c r="E29" t="str">
         <v>-282400</v>
       </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE29" t="str">
+        <v>;X;0;Force</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" t="str" cm="1">
         <f t="array" ref="B30:E30">_xlfn.TEXTSPLIT(A30, ",")</f>
@@ -2227,10 +2326,13 @@
       <c r="E30" t="str">
         <v>-1458100</v>
       </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE30" t="str">
+        <v>;Y;0;Force</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" t="str" cm="1">
         <f t="array" ref="B31:E31">_xlfn.TEXTSPLIT(A31, ",")</f>
@@ -2245,10 +2347,13 @@
       <c r="E31" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE31" t="str">
+        <v>;Z;0;Force</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" t="str" cm="1">
         <f t="array" ref="B32:E32">_xlfn.TEXTSPLIT(A32, ",")</f>
@@ -2263,10 +2368,13 @@
       <c r="E32" t="str">
         <v>140200</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE32" t="str">
+        <v>;Mx;0;Moment</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" t="str" cm="1">
         <f t="array" ref="B33:E33">_xlfn.TEXTSPLIT(A33, ",")</f>
@@ -2281,10 +2389,13 @@
       <c r="E33" t="str">
         <v>-1088100</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE33" t="str">
+        <v>;My;0;Moment</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" t="str" cm="1">
         <f t="array" ref="B34:E34">_xlfn.TEXTSPLIT(A34, ",")</f>
@@ -2299,10 +2410,13 @@
       <c r="E34" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE34" t="str">
+        <v>;X;0;Force</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" t="str" cm="1">
         <f t="array" ref="B35:E35">_xlfn.TEXTSPLIT(A35, ",")</f>
@@ -2317,10 +2431,13 @@
       <c r="E35" t="str">
         <v>-137300</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE35" t="str">
+        <v>;Y;0;Force</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" t="str" cm="1">
         <f t="array" ref="B36:E36">_xlfn.TEXTSPLIT(A36, ",")</f>
@@ -2335,10 +2452,13 @@
       <c r="E36" t="str">
         <v>-1835000</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE36" t="str">
+        <v>;Z;0;Force</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" t="str" cm="1">
         <f t="array" ref="B37:E37">_xlfn.TEXTSPLIT(A37, ",")</f>
@@ -2353,10 +2473,13 @@
       <c r="E37" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE37" t="str">
+        <v>;Mx;0;Moment</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" t="str" cm="1">
         <f t="array" ref="B38:E38">_xlfn.TEXTSPLIT(A38, ",")</f>
@@ -2371,10 +2494,13 @@
       <c r="E38" t="str">
         <v>-113700</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE38" t="str">
+        <v>;My;0;Moment</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" t="str" cm="1">
         <f t="array" ref="B39:E39">_xlfn.TEXTSPLIT(A39, ",")</f>
@@ -2389,10 +2515,13 @@
       <c r="E39" t="str">
         <v>-1445500</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE39" t="str">
+        <v>;X;0;Force</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40" t="str" cm="1">
         <f t="array" ref="B40:E40">_xlfn.TEXTSPLIT(A40, ",")</f>
@@ -2407,10 +2536,13 @@
       <c r="E40" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE40" t="str">
+        <v>;Y;0;Force</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" t="str" cm="1">
         <f t="array" ref="B41:E41">_xlfn.TEXTSPLIT(A41, ",")</f>
@@ -2425,10 +2557,13 @@
       <c r="E41" t="str">
         <v>111300</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE41" t="str">
+        <v>;Z;0;Force</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42" t="str" cm="1">
         <f t="array" ref="B42:E42">_xlfn.TEXTSPLIT(A42, ",")</f>
@@ -2443,10 +2578,13 @@
       <c r="E42" t="str">
         <v>-1526500</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE42" t="str">
+        <v>;Mx;0;Moment</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" t="str" cm="1">
         <f t="array" ref="B43:E43">_xlfn.TEXTSPLIT(A43, ",")</f>
@@ -2461,10 +2599,13 @@
       <c r="E43" t="str">
         <v>320000</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE43" t="str">
+        <v>;My;0;Moment</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44" t="str" cm="1">
         <f t="array" ref="B44:E44">_xlfn.TEXTSPLIT(A44, ",")</f>
@@ -2479,10 +2620,13 @@
       <c r="E44" t="str">
         <v>-320000</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" t="str" cm="1">
         <f t="array" ref="B45:E45">_xlfn.TEXTSPLIT(A45, ",")</f>
@@ -2497,10 +2641,13 @@
       <c r="E45" t="str">
         <v>150000</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46" t="str" cm="1">
         <f t="array" ref="B46:E46">_xlfn.TEXTSPLIT(A46, ",")</f>
@@ -2515,10 +2662,13 @@
       <c r="E46" t="str">
         <v>-150000</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" t="str" cm="1">
         <f t="array" ref="B47:E47">_xlfn.TEXTSPLIT(A47, ",")</f>
@@ -2533,10 +2683,13 @@
       <c r="E47" t="str">
         <v>-1211200</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" t="str" cm="1">
         <f t="array" ref="B48:E48">_xlfn.TEXTSPLIT(A48, ",")</f>
@@ -2551,10 +2704,13 @@
       <c r="E48" t="str">
         <v>-2026000</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" t="str" cm="1">
         <f t="array" ref="B49:E49">_xlfn.TEXTSPLIT(A49, ",")</f>
@@ -2569,10 +2725,13 @@
       <c r="E49" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" t="str" cm="1">
         <f t="array" ref="B50:E50">_xlfn.TEXTSPLIT(A50, ",")</f>
@@ -2587,10 +2746,13 @@
       <c r="E50" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51" t="str" cm="1">
         <f t="array" ref="B51:E51">_xlfn.TEXTSPLIT(A51, ",")</f>
@@ -2605,10 +2767,13 @@
       <c r="E51" t="str">
         <v>371100</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52" t="str" cm="1">
         <f t="array" ref="B52:E52">_xlfn.TEXTSPLIT(A52, ",")</f>
@@ -2623,10 +2788,13 @@
       <c r="E52" t="str">
         <v>-373600</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53" t="str" cm="1">
         <f t="array" ref="B53:E53">_xlfn.TEXTSPLIT(A53, ",")</f>
@@ -2641,10 +2809,13 @@
       <c r="E53" t="str">
         <v>258300</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54" t="str" cm="1">
         <f t="array" ref="B54:E54">_xlfn.TEXTSPLIT(A54, ",")</f>
@@ -2659,10 +2830,13 @@
       <c r="E54" t="str">
         <v>-1224500</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" t="str" cm="1">
         <f t="array" ref="B55:E55">_xlfn.TEXTSPLIT(A55, ",")</f>
@@ -2677,10 +2851,13 @@
       <c r="E55" t="str">
         <v>-1458200</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" t="str" cm="1">
         <f t="array" ref="B56:E56">_xlfn.TEXTSPLIT(A56, ",")</f>
@@ -2695,10 +2872,13 @@
       <c r="E56" t="str">
         <v>-260600.00000000003</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" t="str" cm="1">
         <f t="array" ref="B57:E57">_xlfn.TEXTSPLIT(A57, ",")</f>
@@ -2713,10 +2893,13 @@
       <c r="E57" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" t="str" cm="1">
         <f t="array" ref="B58:E58">_xlfn.TEXTSPLIT(A58, ",")</f>
@@ -2731,10 +2914,13 @@
       <c r="E58" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B59" t="str" cm="1">
         <f t="array" ref="B59:E59">_xlfn.TEXTSPLIT(A59, ",")</f>
@@ -2749,10 +2935,13 @@
       <c r="E59" t="str">
         <v>150000</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B60" t="str" cm="1">
         <f t="array" ref="B60:E60">_xlfn.TEXTSPLIT(A60, ",")</f>
@@ -2767,10 +2956,13 @@
       <c r="E60" t="str">
         <v>-150000</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61" t="str" cm="1">
         <f t="array" ref="B61:E61">_xlfn.TEXTSPLIT(A61, ",")</f>
@@ -2785,10 +2977,13 @@
       <c r="E61" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62" t="str" cm="1">
         <f t="array" ref="B62:E62">_xlfn.TEXTSPLIT(A62, ",")</f>
@@ -2803,10 +2998,13 @@
       <c r="E62" t="str">
         <v>198800</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63" t="str" cm="1">
         <f t="array" ref="B63:E63">_xlfn.TEXTSPLIT(A63, ",")</f>
@@ -2821,10 +3019,13 @@
       <c r="E63" t="str">
         <v>-1220100</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64" t="str" cm="1">
         <f t="array" ref="B64:E64">_xlfn.TEXTSPLIT(A64, ",")</f>
@@ -2839,10 +3040,13 @@
       <c r="E64" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B65" t="str" cm="1">
         <f t="array" ref="B65:E65">_xlfn.TEXTSPLIT(A65, ",")</f>
@@ -2857,10 +3061,13 @@
       <c r="E65" t="str">
         <v>-202000</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B66" t="str" cm="1">
         <f t="array" ref="B66:E66">_xlfn.TEXTSPLIT(A66, ",")</f>
@@ -2875,10 +3082,13 @@
       <c r="E66" t="str">
         <v>-1327200</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B67" t="str" cm="1">
         <f t="array" ref="B67:E67">_xlfn.TEXTSPLIT(A67, ",")</f>
@@ -2893,10 +3103,13 @@
       <c r="E67" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B68" t="str" cm="1">
         <f t="array" ref="B68:E68">_xlfn.TEXTSPLIT(A68, ",")</f>
@@ -2911,10 +3124,13 @@
       <c r="E68" t="str">
         <v>115200</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B69" t="str" cm="1">
         <f t="array" ref="B69:E69">_xlfn.TEXTSPLIT(A69, ",")</f>
@@ -2929,10 +3145,13 @@
       <c r="E69" t="str">
         <v>-1077600</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B70" t="str" cm="1">
         <f t="array" ref="B70:E70">_xlfn.TEXTSPLIT(A70, ",")</f>
@@ -2947,10 +3166,13 @@
       <c r="E70" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B71" t="str" cm="1">
         <f t="array" ref="B71:E71">_xlfn.TEXTSPLIT(A71, ",")</f>
@@ -2965,10 +3187,13 @@
       <c r="E71" t="str">
         <v>-117800</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B72" t="str" cm="1">
         <f t="array" ref="B72:E72">_xlfn.TEXTSPLIT(A72, ",")</f>
@@ -2983,10 +3208,13 @@
       <c r="E72" t="str">
         <v>-1502800</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B73" t="str" cm="1">
         <f t="array" ref="B73:E73">_xlfn.TEXTSPLIT(A73, ",")</f>
@@ -3001,10 +3229,13 @@
       <c r="E73" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B74" t="str" cm="1">
         <f t="array" ref="B74:E74">_xlfn.TEXTSPLIT(A74, ",")</f>
@@ -3019,10 +3250,13 @@
       <c r="E74" t="str">
         <v>-73900</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B75" t="str" cm="1">
         <f t="array" ref="B75:E75">_xlfn.TEXTSPLIT(A75, ",")</f>
@@ -3037,10 +3271,13 @@
       <c r="E75" t="str">
         <v>-1275000</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B76" t="str" cm="1">
         <f t="array" ref="B76:E76">_xlfn.TEXTSPLIT(A76, ",")</f>
@@ -3055,10 +3292,13 @@
       <c r="E76" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B77" t="str" cm="1">
         <f t="array" ref="B77:E77">_xlfn.TEXTSPLIT(A77, ",")</f>
@@ -3073,10 +3313,13 @@
       <c r="E77" t="str">
         <v>71300</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B78" t="str" cm="1">
         <f t="array" ref="B78:E78">_xlfn.TEXTSPLIT(A78, ",")</f>
@@ -3091,10 +3334,13 @@
       <c r="E78" t="str">
         <v>-1354000</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B79" t="str" cm="1">
         <f t="array" ref="B79:E79">_xlfn.TEXTSPLIT(A79, ",")</f>
@@ -3109,10 +3355,13 @@
       <c r="E79" t="str">
         <v>175800</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B80" t="str" cm="1">
         <f t="array" ref="B80:E80">_xlfn.TEXTSPLIT(A80, ",")</f>
@@ -3127,10 +3376,13 @@
       <c r="E80" t="str">
         <v>-1220500</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B81" t="str" cm="1">
         <f t="array" ref="B81:E81">_xlfn.TEXTSPLIT(A81, ",")</f>
@@ -3145,10 +3397,13 @@
       <c r="E81" t="str">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B82" t="str" cm="1">
         <f t="array" ref="B82:E82">_xlfn.TEXTSPLIT(A82, ",")</f>
@@ -3163,10 +3418,13 @@
       <c r="E82" t="str">
         <v>-1327000</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B83" t="str" cm="1">
         <f t="array" ref="B83:E83">_xlfn.TEXTSPLIT(A83, ",")</f>
@@ -3181,10 +3439,13 @@
       <c r="E83" t="str">
         <v>-178900</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="AE83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B84" t="str" cm="1">
         <f t="array" ref="B84:E84">_xlfn.TEXTSPLIT(A84, ",")</f>
@@ -3200,9 +3461,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B85" t="str" cm="1">
         <f t="array" ref="B85:E85">_xlfn.TEXTSPLIT(A85, ",")</f>
@@ -3218,9 +3479,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B86" t="str" cm="1">
         <f t="array" ref="B86:E86">_xlfn.TEXTSPLIT(A86, ",")</f>
@@ -3236,9 +3497,9 @@
         <v>197500</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B87" t="str" cm="1">
         <f t="array" ref="B87:E87">_xlfn.TEXTSPLIT(A87, ",")</f>
@@ -3254,9 +3515,9 @@
         <v>-1029500</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B88" t="str" cm="1">
         <f t="array" ref="B88:E88">_xlfn.TEXTSPLIT(A88, ",")</f>
@@ -3272,9 +3533,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B89" t="str" cm="1">
         <f t="array" ref="B89:E89">_xlfn.TEXTSPLIT(A89, ",")</f>
@@ -3290,9 +3551,9 @@
         <v>-192100</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B90" t="str" cm="1">
         <f t="array" ref="B90:E90">_xlfn.TEXTSPLIT(A90, ",")</f>
@@ -3308,9 +3569,9 @@
         <v>-2519100</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B91" t="str" cm="1">
         <f t="array" ref="B91:E91">_xlfn.TEXTSPLIT(A91, ",")</f>
@@ -3326,9 +3587,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B92" t="str" cm="1">
         <f t="array" ref="B92:E92">_xlfn.TEXTSPLIT(A92, ",")</f>
@@ -3344,9 +3605,9 @@
         <v>-267000</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B93" t="str" cm="1">
         <f t="array" ref="B93:E93">_xlfn.TEXTSPLIT(A93, ",")</f>
@@ -3362,9 +3623,9 @@
         <v>-1504400</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B94" t="str" cm="1">
         <f t="array" ref="B94:E94">_xlfn.TEXTSPLIT(A94, ",")</f>
@@ -3380,9 +3641,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B95" t="str" cm="1">
         <f t="array" ref="B95:E95">_xlfn.TEXTSPLIT(A95, ",")</f>
@@ -3398,9 +3659,9 @@
         <v>264500</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96" t="str" cm="1">
         <f t="array" ref="B96:E96">_xlfn.TEXTSPLIT(A96, ",")</f>
@@ -3418,7 +3679,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B97" t="str" cm="1">
         <f t="array" ref="B97:E97">_xlfn.TEXTSPLIT(A97, ",")</f>
@@ -3436,7 +3697,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B98" t="str" cm="1">
         <f t="array" ref="B98:E98">_xlfn.TEXTSPLIT(A98, ",")</f>
@@ -3454,7 +3715,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B99" t="str" cm="1">
         <f t="array" ref="B99:E99">_xlfn.TEXTSPLIT(A99, ",")</f>
@@ -3472,7 +3733,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B100" t="str" cm="1">
         <f t="array" ref="B100:E100">_xlfn.TEXTSPLIT(A100, ",")</f>
@@ -3490,7 +3751,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B101" t="str" cm="1">
         <f t="array" ref="B101:E101">_xlfn.TEXTSPLIT(A101, ",")</f>
@@ -3508,7 +3769,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B102" t="str" cm="1">
         <f t="array" ref="B102:E102">_xlfn.TEXTSPLIT(A102, ",")</f>
@@ -3526,7 +3787,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B103" t="str" cm="1">
         <f t="array" ref="B103:E103">_xlfn.TEXTSPLIT(A103, ",")</f>
@@ -3544,7 +3805,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B104" t="str" cm="1">
         <f t="array" ref="B104:E104">_xlfn.TEXTSPLIT(A104, ",")</f>
@@ -3562,7 +3823,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B105" t="str" cm="1">
         <f t="array" ref="B105:E105">_xlfn.TEXTSPLIT(A105, ",")</f>
@@ -3580,7 +3841,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B106" t="str" cm="1">
         <f t="array" ref="B106:E106">_xlfn.TEXTSPLIT(A106, ",")</f>
@@ -3598,7 +3859,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B107" t="str" cm="1">
         <f t="array" ref="B107:E107">_xlfn.TEXTSPLIT(A107, ",")</f>
@@ -3616,7 +3877,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B108" t="str" cm="1">
         <f t="array" ref="B108:E108">_xlfn.TEXTSPLIT(A108, ",")</f>
@@ -3634,7 +3895,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B109" t="str" cm="1">
         <f t="array" ref="B109:E109">_xlfn.TEXTSPLIT(A109, ",")</f>
@@ -3652,7 +3913,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B110" t="str" cm="1">
         <f t="array" ref="B110:E110">_xlfn.TEXTSPLIT(A110, ",")</f>
@@ -3670,7 +3931,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B111" t="str" cm="1">
         <f t="array" ref="B111:E111">_xlfn.TEXTSPLIT(A111, ",")</f>
@@ -3688,7 +3949,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B112" t="str" cm="1">
         <f t="array" ref="B112:E112">_xlfn.TEXTSPLIT(A112, ",")</f>
@@ -3706,7 +3967,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B113" t="str" cm="1">
         <f t="array" ref="B113:E113">_xlfn.TEXTSPLIT(A113, ",")</f>
@@ -3724,7 +3985,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B114" t="str" cm="1">
         <f t="array" ref="B114:E114">_xlfn.TEXTSPLIT(A114, ",")</f>
@@ -3742,7 +4003,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B115" t="str" cm="1">
         <f t="array" ref="B115:E115">_xlfn.TEXTSPLIT(A115, ",")</f>
@@ -3760,7 +4021,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B116" t="str" cm="1">
         <f t="array" ref="B116:E116">_xlfn.TEXTSPLIT(A116, ",")</f>
@@ -3778,7 +4039,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B117" t="str" cm="1">
         <f t="array" ref="B117:E117">_xlfn.TEXTSPLIT(A117, ",")</f>
@@ -3796,7 +4057,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B118" t="str" cm="1">
         <f t="array" ref="B118:E118">_xlfn.TEXTSPLIT(A118, ",")</f>
@@ -3814,7 +4075,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B119" t="str" cm="1">
         <f t="array" ref="B119:E119">_xlfn.TEXTSPLIT(A119, ",")</f>
@@ -3832,7 +4093,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B120" t="str" cm="1">
         <f t="array" ref="B120:E120">_xlfn.TEXTSPLIT(A120, ",")</f>
@@ -3850,7 +4111,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B121" t="str" cm="1">
         <f t="array" ref="B121:E121">_xlfn.TEXTSPLIT(A121, ",")</f>
@@ -3868,7 +4129,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B122" t="str" cm="1">
         <f t="array" ref="B122:E122">_xlfn.TEXTSPLIT(A122, ",")</f>
@@ -3886,7 +4147,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B123" t="str" cm="1">
         <f t="array" ref="B123:E123">_xlfn.TEXTSPLIT(A123, ",")</f>
@@ -3904,7 +4165,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B124" t="str" cm="1">
         <f t="array" ref="B124:E124">_xlfn.TEXTSPLIT(A124, ",")</f>
@@ -3922,7 +4183,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B125" t="str" cm="1">
         <f t="array" ref="B125:E125">_xlfn.TEXTSPLIT(A125, ",")</f>
@@ -3940,7 +4201,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B126" t="str" cm="1">
         <f t="array" ref="B126:E126">_xlfn.TEXTSPLIT(A126, ",")</f>
@@ -3958,7 +4219,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B127" t="str" cm="1">
         <f t="array" ref="B127:E127">_xlfn.TEXTSPLIT(A127, ",")</f>
@@ -3976,7 +4237,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B128" t="str" cm="1">
         <f t="array" ref="B128:E128">_xlfn.TEXTSPLIT(A128, ",")</f>
@@ -3994,7 +4255,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B129" t="str" cm="1">
         <f t="array" ref="B129:E129">_xlfn.TEXTSPLIT(A129, ",")</f>
@@ -4012,7 +4273,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B130" t="str" cm="1">
         <f t="array" ref="B130:E130">_xlfn.TEXTSPLIT(A130, ",")</f>
@@ -4030,7 +4291,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B131" t="str" cm="1">
         <f t="array" ref="B131:E131">_xlfn.TEXTSPLIT(A131, ",")</f>
@@ -4048,7 +4309,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B132" t="str" cm="1">
         <f t="array" ref="B132:E132">_xlfn.TEXTSPLIT(A132, ",")</f>
@@ -4066,7 +4327,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B133" t="str" cm="1">
         <f t="array" ref="B133:E133">_xlfn.TEXTSPLIT(A133, ",")</f>
@@ -4084,7 +4345,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B134" t="str" cm="1">
         <f t="array" ref="B134:E134">_xlfn.TEXTSPLIT(A134, ",")</f>
@@ -4102,7 +4363,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B135" t="str" cm="1">
         <f t="array" ref="B135:E135">_xlfn.TEXTSPLIT(A135, ",")</f>
@@ -4120,7 +4381,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B136" t="str" cm="1">
         <f t="array" ref="B136:E136">_xlfn.TEXTSPLIT(A136, ",")</f>
@@ -4138,7 +4399,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B137" t="str" cm="1">
         <f t="array" ref="B137:E137">_xlfn.TEXTSPLIT(A137, ",")</f>
@@ -4156,7 +4417,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B138" t="str" cm="1">
         <f t="array" ref="B138:E138">_xlfn.TEXTSPLIT(A138, ",")</f>
@@ -4174,7 +4435,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B139" t="str" cm="1">
         <f t="array" ref="B139:E139">_xlfn.TEXTSPLIT(A139, ",")</f>
@@ -4192,7 +4453,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B140" t="str" cm="1">
         <f t="array" ref="B140:E140">_xlfn.TEXTSPLIT(A140, ",")</f>
@@ -4210,7 +4471,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B141" t="str" cm="1">
         <f t="array" ref="B141:E141">_xlfn.TEXTSPLIT(A141, ",")</f>
@@ -4228,7 +4489,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B142" t="str" cm="1">
         <f t="array" ref="B142:E142">_xlfn.TEXTSPLIT(A142, ",")</f>
@@ -4246,7 +4507,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B143" t="str" cm="1">
         <f t="array" ref="B143:E143">_xlfn.TEXTSPLIT(A143, ",")</f>
@@ -4264,7 +4525,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B144" t="str" cm="1">
         <f t="array" ref="B144:E144">_xlfn.TEXTSPLIT(A144, ",")</f>
@@ -4282,7 +4543,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B145" t="str" cm="1">
         <f t="array" ref="B145:E145">_xlfn.TEXTSPLIT(A145, ",")</f>
@@ -4300,7 +4561,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B146" t="str" cm="1">
         <f t="array" ref="B146:E146">_xlfn.TEXTSPLIT(A146, ",")</f>
@@ -4318,7 +4579,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B147" t="str" cm="1">
         <f t="array" ref="B147:E147">_xlfn.TEXTSPLIT(A147, ",")</f>
@@ -4336,7 +4597,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B148" t="str" cm="1">
         <f t="array" ref="B148:E148">_xlfn.TEXTSPLIT(A148, ",")</f>
@@ -4354,7 +4615,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B149" t="str" cm="1">
         <f t="array" ref="B149:E149">_xlfn.TEXTSPLIT(A149, ",")</f>
@@ -4372,7 +4633,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B150" t="str" cm="1">
         <f t="array" ref="B150:E150">_xlfn.TEXTSPLIT(A150, ",")</f>
@@ -4390,7 +4651,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B151" t="str" cm="1">
         <f t="array" ref="B151:E151">_xlfn.TEXTSPLIT(A151, ",")</f>
@@ -4408,7 +4669,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B152" t="str" cm="1">
         <f t="array" ref="B152:E152">_xlfn.TEXTSPLIT(A152, ",")</f>
@@ -4426,7 +4687,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B153" t="str" cm="1">
         <f t="array" ref="B153:E153">_xlfn.TEXTSPLIT(A153, ",")</f>
@@ -4444,7 +4705,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B154" t="str" cm="1">
         <f t="array" ref="B154:E154">_xlfn.TEXTSPLIT(A154, ",")</f>
@@ -4462,7 +4723,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B155" t="str" cm="1">
         <f t="array" ref="B155:E155">_xlfn.TEXTSPLIT(A155, ",")</f>
@@ -4480,7 +4741,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B156" t="str" cm="1">
         <f t="array" ref="B156:E156">_xlfn.TEXTSPLIT(A156, ",")</f>
@@ -4498,7 +4759,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B157" t="str" cm="1">
         <f t="array" ref="B157:E157">_xlfn.TEXTSPLIT(A157, ",")</f>
@@ -4516,7 +4777,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B158" t="str" cm="1">
         <f t="array" ref="B158:E158">_xlfn.TEXTSPLIT(A158, ",")</f>
@@ -4534,7 +4795,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B159" t="str" cm="1">
         <f t="array" ref="B159:E159">_xlfn.TEXTSPLIT(A159, ",")</f>
@@ -4552,7 +4813,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B160" t="str" cm="1">
         <f t="array" ref="B160:E160">_xlfn.TEXTSPLIT(A160, ",")</f>
@@ -4570,7 +4831,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B161" t="str" cm="1">
         <f t="array" ref="B161:E161">_xlfn.TEXTSPLIT(A161, ",")</f>
@@ -4588,7 +4849,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B162" t="str" cm="1">
         <f t="array" ref="B162:E162">_xlfn.TEXTSPLIT(A162, ",")</f>
@@ -4606,7 +4867,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B163" t="str" cm="1">
         <f t="array" ref="B163:E163">_xlfn.TEXTSPLIT(A163, ",")</f>
@@ -4624,7 +4885,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B164" t="str" cm="1">
         <f t="array" ref="B164:E164">_xlfn.TEXTSPLIT(A164, ",")</f>
@@ -4642,7 +4903,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B165" t="str" cm="1">
         <f t="array" ref="B165:E165">_xlfn.TEXTSPLIT(A165, ",")</f>
@@ -4660,7 +4921,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B166" t="str" cm="1">
         <f t="array" ref="B166:E166">_xlfn.TEXTSPLIT(A166, ",")</f>
@@ -4678,7 +4939,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B167" t="str" cm="1">
         <f t="array" ref="B167:E167">_xlfn.TEXTSPLIT(A167, ",")</f>
@@ -4696,7 +4957,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B168" t="str" cm="1">
         <f t="array" ref="B168:E168">_xlfn.TEXTSPLIT(A168, ",")</f>
@@ -4714,7 +4975,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B169" t="str" cm="1">
         <f t="array" ref="B169:E169">_xlfn.TEXTSPLIT(A169, ",")</f>
@@ -4732,7 +4993,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B170" t="str" cm="1">
         <f t="array" ref="B170:E170">_xlfn.TEXTSPLIT(A170, ",")</f>
@@ -4750,7 +5011,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B171" t="str" cm="1">
         <f t="array" ref="B171:E171">_xlfn.TEXTSPLIT(A171, ",")</f>
@@ -4768,7 +5029,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B172" t="str" cm="1">
         <f t="array" ref="B172:E172">_xlfn.TEXTSPLIT(A172, ",")</f>
@@ -4786,7 +5047,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B173" t="str" cm="1">
         <f t="array" ref="B173:E173">_xlfn.TEXTSPLIT(A173, ",")</f>
@@ -4804,7 +5065,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B174" t="str" cm="1">
         <f t="array" ref="B174:E174">_xlfn.TEXTSPLIT(A174, ",")</f>
@@ -4822,7 +5083,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B175" t="str" cm="1">
         <f t="array" ref="B175:E175">_xlfn.TEXTSPLIT(A175, ",")</f>
@@ -4840,7 +5101,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B176" t="str" cm="1">
         <f t="array" ref="B176:E176">_xlfn.TEXTSPLIT(A176, ",")</f>
@@ -4858,7 +5119,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B177" t="str" cm="1">
         <f t="array" ref="B177:E177">_xlfn.TEXTSPLIT(A177, ",")</f>
@@ -4876,7 +5137,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B178" t="str" cm="1">
         <f t="array" ref="B178:E178">_xlfn.TEXTSPLIT(A178, ",")</f>
@@ -4894,7 +5155,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B179" t="str" cm="1">
         <f t="array" ref="B179:E179">_xlfn.TEXTSPLIT(A179, ",")</f>
@@ -4912,7 +5173,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B180" t="str" cm="1">
         <f t="array" ref="B180:E180">_xlfn.TEXTSPLIT(A180, ",")</f>
@@ -4930,7 +5191,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B181" t="str" cm="1">
         <f t="array" ref="B181:E181">_xlfn.TEXTSPLIT(A181, ",")</f>
@@ -4948,7 +5209,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B182" t="str" cm="1">
         <f t="array" ref="B182:E182">_xlfn.TEXTSPLIT(A182, ",")</f>
@@ -4966,7 +5227,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B183" t="str" cm="1">
         <f t="array" ref="B183:E183">_xlfn.TEXTSPLIT(A183, ",")</f>
@@ -4984,7 +5245,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B184" t="str" cm="1">
         <f t="array" ref="B184:E184">_xlfn.TEXTSPLIT(A184, ",")</f>
@@ -5002,7 +5263,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B185" t="str" cm="1">
         <f t="array" ref="B185:E185">_xlfn.TEXTSPLIT(A185, ",")</f>
@@ -5020,7 +5281,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B186" t="str" cm="1">
         <f t="array" ref="B186:E186">_xlfn.TEXTSPLIT(A186, ",")</f>
@@ -5038,7 +5299,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B187" t="str" cm="1">
         <f t="array" ref="B187:E187">_xlfn.TEXTSPLIT(A187, ",")</f>
@@ -5056,7 +5317,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B188" t="str" cm="1">
         <f t="array" ref="B188:E188">_xlfn.TEXTSPLIT(A188, ",")</f>
@@ -5074,7 +5335,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B189" t="str" cm="1">
         <f t="array" ref="B189:E189">_xlfn.TEXTSPLIT(A189, ",")</f>
@@ -5092,7 +5353,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B190" t="str" cm="1">
         <f t="array" ref="B190:E190">_xlfn.TEXTSPLIT(A190, ",")</f>
@@ -5110,7 +5371,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B191" t="str" cm="1">
         <f t="array" ref="B191:E191">_xlfn.TEXTSPLIT(A191, ",")</f>
@@ -5128,7 +5389,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B192" t="str" cm="1">
         <f t="array" ref="B192:E192">_xlfn.TEXTSPLIT(A192, ",")</f>
@@ -5146,7 +5407,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B193" t="str" cm="1">
         <f t="array" ref="B193:E193">_xlfn.TEXTSPLIT(A193, ",")</f>
@@ -5164,7 +5425,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B194" t="str" cm="1">
         <f t="array" ref="B194:E194">_xlfn.TEXTSPLIT(A194, ",")</f>
@@ -5182,7 +5443,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B195" t="str" cm="1">
         <f t="array" ref="B195:E195">_xlfn.TEXTSPLIT(A195, ",")</f>
@@ -5200,7 +5461,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B196" t="str" cm="1">
         <f t="array" ref="B196:E196">_xlfn.TEXTSPLIT(A196, ",")</f>
@@ -5218,7 +5479,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B197" t="str" cm="1">
         <f t="array" ref="B197:E197">_xlfn.TEXTSPLIT(A197, ",")</f>
@@ -5236,7 +5497,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B198" t="str" cm="1">
         <f t="array" ref="B198:E198">_xlfn.TEXTSPLIT(A198, ",")</f>
@@ -5254,7 +5515,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B199" t="str" cm="1">
         <f t="array" ref="B199:E199">_xlfn.TEXTSPLIT(A199, ",")</f>
@@ -5272,7 +5533,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B200" t="str" cm="1">
         <f t="array" ref="B200:E200">_xlfn.TEXTSPLIT(A200, ",")</f>
@@ -5290,7 +5551,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B201" t="str" cm="1">
         <f t="array" ref="B201:E201">_xlfn.TEXTSPLIT(A201, ",")</f>
@@ -5308,7 +5569,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B202" t="str" cm="1">
         <f t="array" ref="B202:E202">_xlfn.TEXTSPLIT(A202, ",")</f>
@@ -5326,7 +5587,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B203" t="str" cm="1">
         <f t="array" ref="B203:E203">_xlfn.TEXTSPLIT(A203, ",")</f>
@@ -5344,7 +5605,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B204" t="str" cm="1">
         <f t="array" ref="B204:E204">_xlfn.TEXTSPLIT(A204, ",")</f>
@@ -5362,7 +5623,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B205" t="str" cm="1">
         <f t="array" ref="B205:E205">_xlfn.TEXTSPLIT(A205, ",")</f>
@@ -5380,7 +5641,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B206" t="str" cm="1">
         <f t="array" ref="B206:E206">_xlfn.TEXTSPLIT(A206, ",")</f>
@@ -5398,7 +5659,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B207" t="str" cm="1">
         <f t="array" ref="B207:E207">_xlfn.TEXTSPLIT(A207, ",")</f>
@@ -5416,7 +5677,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B208" t="str" cm="1">
         <f t="array" ref="B208:E208">_xlfn.TEXTSPLIT(A208, ",")</f>
@@ -5434,7 +5695,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B209" t="str" cm="1">
         <f t="array" ref="B209:E209">_xlfn.TEXTSPLIT(A209, ",")</f>
@@ -5452,7 +5713,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B210" t="str" cm="1">
         <f t="array" ref="B210:E210">_xlfn.TEXTSPLIT(A210, ",")</f>
@@ -5470,7 +5731,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B211" t="str" cm="1">
         <f t="array" ref="B211:E211">_xlfn.TEXTSPLIT(A211, ",")</f>
@@ -5488,7 +5749,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B212" t="str" cm="1">
         <f t="array" ref="B212:E212">_xlfn.TEXTSPLIT(A212, ",")</f>
@@ -5506,7 +5767,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B213" t="str" cm="1">
         <f t="array" ref="B213:E213">_xlfn.TEXTSPLIT(A213, ",")</f>
@@ -5524,7 +5785,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B214" t="str" cm="1">
         <f t="array" ref="B214:E214">_xlfn.TEXTSPLIT(A214, ",")</f>
@@ -5542,7 +5803,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B215" t="str" cm="1">
         <f t="array" ref="B215:E215">_xlfn.TEXTSPLIT(A215, ",")</f>
@@ -5560,7 +5821,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B216" t="str" cm="1">
         <f t="array" ref="B216:E216">_xlfn.TEXTSPLIT(A216, ",")</f>
@@ -5578,7 +5839,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B217" t="str" cm="1">
         <f t="array" ref="B217:E217">_xlfn.TEXTSPLIT(A217, ",")</f>
@@ -5596,7 +5857,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B218" t="str" cm="1">
         <f t="array" ref="B218:E218">_xlfn.TEXTSPLIT(A218, ",")</f>
@@ -5614,7 +5875,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B219" t="str" cm="1">
         <f t="array" ref="B219:E219">_xlfn.TEXTSPLIT(A219, ",")</f>
@@ -5632,7 +5893,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B220" t="str" cm="1">
         <f t="array" ref="B220:E220">_xlfn.TEXTSPLIT(A220, ",")</f>
@@ -5650,7 +5911,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B221" t="str" cm="1">
         <f t="array" ref="B221:E221">_xlfn.TEXTSPLIT(A221, ",")</f>
@@ -5668,7 +5929,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B222" t="str" cm="1">
         <f t="array" ref="B222:E222">_xlfn.TEXTSPLIT(A222, ",")</f>
@@ -5686,7 +5947,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B223" t="str" cm="1">
         <f t="array" ref="B223:E223">_xlfn.TEXTSPLIT(A223, ",")</f>
@@ -5704,7 +5965,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B224" t="str" cm="1">
         <f t="array" ref="B224:E224">_xlfn.TEXTSPLIT(A224, ",")</f>
@@ -5722,7 +5983,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B225" t="str" cm="1">
         <f t="array" ref="B225:E225">_xlfn.TEXTSPLIT(A225, ",")</f>
@@ -5740,7 +6001,7 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B226" t="str" cm="1">
         <f t="array" ref="B226:E226">_xlfn.TEXTSPLIT(A226, ",")</f>
@@ -5758,7 +6019,7 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B227" t="str" cm="1">
         <f t="array" ref="B227:E227">_xlfn.TEXTSPLIT(A227, ",")</f>
@@ -5776,7 +6037,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B228" t="str" cm="1">
         <f t="array" ref="B228:E228">_xlfn.TEXTSPLIT(A228, ",")</f>
@@ -5794,7 +6055,7 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B229" t="str" cm="1">
         <f t="array" ref="B229:E229">_xlfn.TEXTSPLIT(A229, ",")</f>
@@ -5812,7 +6073,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B230" t="str" cm="1">
         <f t="array" ref="B230:E230">_xlfn.TEXTSPLIT(A230, ",")</f>
@@ -5830,7 +6091,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B231" t="str" cm="1">
         <f t="array" ref="B231:E231">_xlfn.TEXTSPLIT(A231, ",")</f>
@@ -5848,7 +6109,7 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B232" t="str" cm="1">
         <f t="array" ref="B232:E232">_xlfn.TEXTSPLIT(A232, ",")</f>
@@ -5866,7 +6127,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B233" t="str" cm="1">
         <f t="array" ref="B233:E233">_xlfn.TEXTSPLIT(A233, ",")</f>
@@ -5884,7 +6145,7 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B234" t="str" cm="1">
         <f t="array" ref="B234:E234">_xlfn.TEXTSPLIT(A234, ",")</f>
@@ -5902,7 +6163,7 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B235" t="str" cm="1">
         <f t="array" ref="B235:E235">_xlfn.TEXTSPLIT(A235, ",")</f>
@@ -5920,7 +6181,7 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B236" t="str" cm="1">
         <f t="array" ref="B236:E236">_xlfn.TEXTSPLIT(A236, ",")</f>
@@ -5938,7 +6199,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B237" t="str" cm="1">
         <f t="array" ref="B237:E237">_xlfn.TEXTSPLIT(A237, ",")</f>
@@ -5956,7 +6217,7 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B238" t="str" cm="1">
         <f t="array" ref="B238:E238">_xlfn.TEXTSPLIT(A238, ",")</f>
@@ -5974,7 +6235,7 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B239" t="str" cm="1">
         <f t="array" ref="B239:E239">_xlfn.TEXTSPLIT(A239, ",")</f>
@@ -5992,7 +6253,7 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B240" t="str" cm="1">
         <f t="array" ref="B240:E240">_xlfn.TEXTSPLIT(A240, ",")</f>
@@ -6010,7 +6271,7 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B241" t="str" cm="1">
         <f t="array" ref="B241:E241">_xlfn.TEXTSPLIT(A241, ",")</f>
@@ -6028,7 +6289,7 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B242" t="str" cm="1">
         <f t="array" ref="B242:E242">_xlfn.TEXTSPLIT(A242, ",")</f>
@@ -6046,7 +6307,7 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B243" t="str" cm="1">
         <f t="array" ref="B243:E243">_xlfn.TEXTSPLIT(A243, ",")</f>
@@ -6064,7 +6325,7 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B244" t="str" cm="1">
         <f t="array" ref="B244:E244">_xlfn.TEXTSPLIT(A244, ",")</f>
@@ -6082,7 +6343,7 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B245" t="str" cm="1">
         <f t="array" ref="B245:E245">_xlfn.TEXTSPLIT(A245, ",")</f>
@@ -6100,7 +6361,7 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B246" t="str" cm="1">
         <f t="array" ref="B246:E246">_xlfn.TEXTSPLIT(A246, ",")</f>
@@ -6118,7 +6379,7 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B247" t="str" cm="1">
         <f t="array" ref="B247:E247">_xlfn.TEXTSPLIT(A247, ",")</f>
@@ -6136,7 +6397,7 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B248" t="str" cm="1">
         <f t="array" ref="B248:E248">_xlfn.TEXTSPLIT(A248, ",")</f>
@@ -6154,7 +6415,7 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B249" t="str" cm="1">
         <f t="array" ref="B249:E249">_xlfn.TEXTSPLIT(A249, ",")</f>
@@ -6172,7 +6433,7 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B250" t="str" cm="1">
         <f t="array" ref="B250:E250">_xlfn.TEXTSPLIT(A250, ",")</f>
@@ -6190,7 +6451,7 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B251" t="str" cm="1">
         <f t="array" ref="B251:E251">_xlfn.TEXTSPLIT(A251, ",")</f>
@@ -6208,7 +6469,7 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B252" t="str" cm="1">
         <f t="array" ref="B252:E252">_xlfn.TEXTSPLIT(A252, ",")</f>
@@ -6226,7 +6487,7 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B253" t="str" cm="1">
         <f t="array" ref="B253:E253">_xlfn.TEXTSPLIT(A253, ",")</f>
@@ -6244,7 +6505,7 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B254" t="str" cm="1">
         <f t="array" ref="B254:E254">_xlfn.TEXTSPLIT(A254, ",")</f>
@@ -6262,7 +6523,7 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B255" t="str" cm="1">
         <f t="array" ref="B255:E255">_xlfn.TEXTSPLIT(A255, ",")</f>
@@ -6280,7 +6541,7 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B256" t="str" cm="1">
         <f t="array" ref="B256:E256">_xlfn.TEXTSPLIT(A256, ",")</f>
@@ -6298,7 +6559,7 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B257" t="str" cm="1">
         <f t="array" ref="B257:E257">_xlfn.TEXTSPLIT(A257, ",")</f>
@@ -6316,7 +6577,7 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B258" t="str" cm="1">
         <f t="array" ref="B258:E258">_xlfn.TEXTSPLIT(A258, ",")</f>
@@ -6334,7 +6595,7 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B259" t="str" cm="1">
         <f t="array" ref="B259:E259">_xlfn.TEXTSPLIT(A259, ",")</f>
@@ -6352,7 +6613,7 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B260" t="str" cm="1">
         <f t="array" ref="B260:E260">_xlfn.TEXTSPLIT(A260, ",")</f>
@@ -6370,7 +6631,7 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B261" t="str" cm="1">
         <f t="array" ref="B261:E261">_xlfn.TEXTSPLIT(A261, ",")</f>
@@ -6388,7 +6649,7 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B262" t="str" cm="1">
         <f t="array" ref="B262:E262">_xlfn.TEXTSPLIT(A262, ",")</f>
@@ -6406,7 +6667,7 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B263" t="str" cm="1">
         <f t="array" ref="B263:E263">_xlfn.TEXTSPLIT(A263, ",")</f>
@@ -6424,7 +6685,7 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B264" t="str" cm="1">
         <f t="array" ref="B264:E264">_xlfn.TEXTSPLIT(A264, ",")</f>
@@ -6442,7 +6703,7 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B265" t="str" cm="1">
         <f t="array" ref="B265:E265">_xlfn.TEXTSPLIT(A265, ",")</f>
@@ -6460,7 +6721,7 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B266" t="str" cm="1">
         <f t="array" ref="B266:E266">_xlfn.TEXTSPLIT(A266, ",")</f>
@@ -6478,7 +6739,7 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B267" t="str" cm="1">
         <f t="array" ref="B267:E267">_xlfn.TEXTSPLIT(A267, ",")</f>
@@ -6496,7 +6757,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B268" t="str" cm="1">
         <f t="array" ref="B268:E268">_xlfn.TEXTSPLIT(A268, ",")</f>
@@ -6514,7 +6775,7 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B269" t="str" cm="1">
         <f t="array" ref="B269:E269">_xlfn.TEXTSPLIT(A269, ",")</f>
@@ -6532,7 +6793,7 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B270" t="str" cm="1">
         <f t="array" ref="B270:E270">_xlfn.TEXTSPLIT(A270, ",")</f>
@@ -6550,7 +6811,7 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B271" t="str" cm="1">
         <f t="array" ref="B271:E271">_xlfn.TEXTSPLIT(A271, ",")</f>
@@ -6568,7 +6829,7 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B272" t="str" cm="1">
         <f t="array" ref="B272:E272">_xlfn.TEXTSPLIT(A272, ",")</f>
@@ -6586,7 +6847,7 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B273" t="str" cm="1">
         <f t="array" ref="B273:E273">_xlfn.TEXTSPLIT(A273, ",")</f>
@@ -6604,7 +6865,7 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B274" t="str" cm="1">
         <f t="array" ref="B274:E274">_xlfn.TEXTSPLIT(A274, ",")</f>
@@ -6622,7 +6883,7 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B275" t="str" cm="1">
         <f t="array" ref="B275:E275">_xlfn.TEXTSPLIT(A275, ",")</f>
@@ -6640,7 +6901,7 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B276" t="str" cm="1">
         <f t="array" ref="B276:E276">_xlfn.TEXTSPLIT(A276, ",")</f>
@@ -6658,7 +6919,7 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B277" t="str" cm="1">
         <f t="array" ref="B277:E277">_xlfn.TEXTSPLIT(A277, ",")</f>
@@ -6676,7 +6937,7 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B278" t="str" cm="1">
         <f t="array" ref="B278:E278">_xlfn.TEXTSPLIT(A278, ",")</f>
@@ -6708,7 +6969,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6718,15 +6984,14 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100BA85B17551307B4383D2980D4EFA5515" ma:contentTypeVersion="12" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="57aaa53a121281638ac8bc132f802243">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="173d6b2f-59a8-488e-935d-67e78bda59e5" xmlns:ns3="b97dc65e-fe16-4df7-925c-ff3316bf7bf3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="141727366efbfc4d0736cea1f099176a" ns2:_="" ns3:_="">
     <xsd:import namespace="173d6b2f-59a8-488e-935d-67e78bda59e5"/>
@@ -6943,13 +7208,11 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69C2894E-68C9-476D-803E-814AC6EBDDB7}">
-  <ds:schemaRefs/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
@@ -6964,14 +7227,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69C2894E-68C9-476D-803E-814AC6EBDDB7}">
+  <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{754B3D83-15E4-4B5F-8568-57884EBAF882}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6988,10 +7255,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
I updated the comments
</commit_message>
<xml_diff>
--- a/phases.xlsx
+++ b/phases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57E010A-9C9C-40DD-B6A5-5C8719CEB990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC05789-7DAD-472C-85E1-6F78C6639B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="292">
   <si>
     <t>BG2,X,Force,1000000</t>
   </si>
@@ -948,6 +948,9 @@
   </si>
   <si>
     <t>BG10</t>
+  </si>
+  <si>
+    <t>Phase 2: Which load cases do you want?</t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1314,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:AE278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="AA23" sqref="AA23"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1336,6 +1339,9 @@
       <c r="A1" t="s">
         <v>286</v>
       </c>
+      <c r="H1" t="s">
+        <v>291</v>
+      </c>
       <c r="P1" t="s">
         <v>283</v>
       </c>
@@ -6969,29 +6975,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100BA85B17551307B4383D2980D4EFA5515" ma:contentTypeVersion="12" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="57aaa53a121281638ac8bc132f802243">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="173d6b2f-59a8-488e-935d-67e78bda59e5" xmlns:ns3="b97dc65e-fe16-4df7-925c-ff3316bf7bf3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="141727366efbfc4d0736cea1f099176a" ns2:_="" ns3:_="">
     <xsd:import namespace="173d6b2f-59a8-488e-935d-67e78bda59e5"/>
@@ -7208,37 +7191,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Sweco\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BD3FF0-C90B-4BBB-AF14-2B7944CED71E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fe0e463f-46c1-4b5a-aeae-2e65b5901510"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69C2894E-68C9-476D-803E-814AC6EBDDB7}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{754B3D83-15E4-4B5F-8568-57884EBAF882}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7255,4 +7231,34 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDE50B2-2507-4A17-8842-A7EE75090943}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69C2894E-68C9-476D-803E-814AC6EBDDB7}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BD3FF0-C90B-4BBB-AF14-2B7944CED71E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fe0e463f-46c1-4b5a-aeae-2e65b5901510"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B094B8C0-0888-4622-A87D-10D4D23C20D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>